<commit_message>
deleted:    .Rhistory 	modified:   .gitignore 	modified:   LLM dataset and training/LLM training.ipynb 	modified:   LLM dataset and training/LLM_question_dataset.xlsx 	new file:   LLM dataset and training/label_encoder.pkl 	new file:   LLM dataset and training/tokenizer.pkl
</commit_message>
<xml_diff>
--- a/LLM dataset and training/LLM_question_dataset.xlsx
+++ b/LLM dataset and training/LLM_question_dataset.xlsx
@@ -841,7 +841,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -930,7 +930,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="129.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.22"/>
@@ -3180,10 +3180,10 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="118.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.22"/>

</xml_diff>